<commit_message>
Rewriting the load structure of df's --> now based on header files
</commit_message>
<xml_diff>
--- a/Data/MonthlyHeaderMapping.xlsx
+++ b/Data/MonthlyHeaderMapping.xlsx
@@ -212,18 +212,9 @@
     <t>Borrower_Assistance_Status_Code</t>
   </si>
   <si>
-    <t>dtype</t>
-  </si>
-  <si>
-    <t>np.float_ </t>
-  </si>
-  <si>
     <t>str</t>
   </si>
   <si>
-    <t>np.float_</t>
-  </si>
-  <si>
     <t>str </t>
   </si>
   <si>
@@ -231,6 +222,15 @@
   </si>
   <si>
     <t>ColumnPosition</t>
+  </si>
+  <si>
+    <t>numpy.float_ </t>
+  </si>
+  <si>
+    <t>numpy.float_</t>
+  </si>
+  <si>
+    <t>dType</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -582,7 +582,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -596,7 +596,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <f>D2+1</f>
@@ -611,7 +611,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D31" si="0">D3+1</f>
@@ -626,7 +626,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -641,7 +641,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -656,7 +656,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -671,7 +671,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -686,7 +686,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -701,7 +701,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -716,7 +716,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -731,7 +731,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -746,7 +746,7 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -761,7 +761,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -776,7 +776,7 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -791,7 +791,7 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -806,7 +806,7 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -821,7 +821,7 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -836,7 +836,7 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -851,7 +851,7 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -866,7 +866,7 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
@@ -881,7 +881,7 @@
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
@@ -896,7 +896,7 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
@@ -911,7 +911,7 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
@@ -926,7 +926,7 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
@@ -941,7 +941,7 @@
         <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
@@ -956,7 +956,7 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
@@ -971,7 +971,7 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
@@ -986,7 +986,7 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
@@ -1001,7 +1001,7 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
@@ -1016,7 +1016,7 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>

</xml_diff>